<commit_message>
Commiting after adding category in report
</commit_message>
<xml_diff>
--- a/src/TestData/Automation_Module_Driver_Excel.xlsx
+++ b/src/TestData/Automation_Module_Driver_Excel.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="AutomationModules" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Info" sheetId="2" r:id="rId1"/>
+    <sheet name="AutomationModules" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>TMID</t>
   </si>
@@ -54,7 +54,25 @@
     <t>Add_Appointment</t>
   </si>
   <si>
-    <t>Utility</t>
+    <t>Login into Facebook</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>HostName</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Aman</t>
+  </si>
+  <si>
+    <t>Aman Mehndiratta</t>
   </si>
 </sst>
 </file>
@@ -386,10 +404,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -440,31 +500,14 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commiting with some changes regarding static objects in class execute. and correctly working extent report.
</commit_message>
<xml_diff>
--- a/src/TestData/Automation_Module_Driver_Excel.xlsx
+++ b/src/TestData/Automation_Module_Driver_Excel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>TMID</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Add_Appointment</t>
   </si>
   <si>
-    <t>Login into Facebook</t>
-  </si>
-  <si>
     <t>Environment</t>
   </si>
   <si>
@@ -76,6 +73,12 @@
   </si>
   <si>
     <t>Author</t>
+  </si>
+  <si>
+    <t>Login_into_EMR</t>
+  </si>
+  <si>
+    <t>Registration</t>
   </si>
 </sst>
 </file>
@@ -436,24 +439,24 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -467,7 +470,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -493,7 +496,7 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -510,18 +513,24 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -529,16 +538,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added functionality in report config class to add system MAC address in report
</commit_message>
<xml_diff>
--- a/src/TestData/Automation_Module_Driver_Excel.xlsx
+++ b/src/TestData/Automation_Module_Driver_Excel.xlsx
@@ -470,7 +470,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -544,7 +544,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>

</xml_diff>